<commit_message>
responsive img via src set ou css pour les banner, minify the js, change color of text
</commit_message>
<xml_diff>
--- a/Audit-SEO.xlsx
+++ b/Audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Samuel/Desktop/P4_Prigent_Samuel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A789A4C6-F630-9B49-900F-D93974B37F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FA40AB-5D4A-E049-8BE6-F848D4D6EF67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="620" windowWidth="28760" windowHeight="17380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="92">
   <si>
     <t>Catégorie</t>
   </si>
@@ -272,6 +272,66 @@
   </si>
   <si>
     <t>les images était trop petite sur grand écran car le conteneur ne pouvait pas s'élargir plus que 600px</t>
+  </si>
+  <si>
+    <t>Le focus des nav en transparent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l'effet était déjà réglés il fallait enlever le transparent </t>
+  </si>
+  <si>
+    <t>Tab ordre de selection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j'ai enlever le logo du site comme selectable par tab </t>
+  </si>
+  <si>
+    <t xml:space="preserve">taille label formulaire </t>
+  </si>
+  <si>
+    <t>a été augmenté</t>
+  </si>
+  <si>
+    <t>Un br était présent à la fin de la phrase du dernier texte mais ce n'est pas très lisible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">je met ce qui était entre paranthèse en place holder dans la case </t>
+  </si>
+  <si>
+    <t>Le input de comment nous avait vous connu était en email</t>
+  </si>
+  <si>
+    <t>je l'ai remis en message</t>
+  </si>
+  <si>
+    <t>SEO</t>
+  </si>
+  <si>
+    <t>ajout d'une description</t>
+  </si>
+  <si>
+    <t>mots clés</t>
+  </si>
+  <si>
+    <t>paris dans les mots clés alors que l'agence est à lyon</t>
+  </si>
+  <si>
+    <t>Pas de méta description et mots clés sur la page contact</t>
+  </si>
+  <si>
+    <t>pas de méta description du content sur la page d'acceuil</t>
+  </si>
+  <si>
+    <t>Taille fichiers temps de chargement</t>
+  </si>
+  <si>
+    <t>fichiers JS non minifier</t>
+  </si>
+  <si>
+    <t>ajout de la fonction async</t>
+  </si>
+  <si>
+    <t>pour ne pas que le js bloque le rendu du reste le async n'a pas été mis sur les boutons car il bougeait la mise en page</t>
   </si>
 </sst>
 </file>
@@ -669,13 +729,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W1004"/>
+  <dimension ref="A1:W203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" style="6" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" style="6" customWidth="1"/>
@@ -684,7 +744,7 @@
     <col min="24" max="16384" width="11.28515625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="3" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1029,1637 +1089,876 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="40" x14ac:dyDescent="0.2">
       <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="20" x14ac:dyDescent="0.2">
       <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="20" x14ac:dyDescent="0.2">
       <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="40" x14ac:dyDescent="0.2">
       <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-    </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A43" s="14"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
     </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="20" x14ac:dyDescent="0.2">
       <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
+      <c r="B44" s="14" t="s">
+        <v>82</v>
+      </c>
       <c r="C44" s="14"/>
     </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="40" x14ac:dyDescent="0.2">
       <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="20" x14ac:dyDescent="0.2">
       <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="40" x14ac:dyDescent="0.2">
       <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
+      <c r="B47" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="C47" s="14"/>
     </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A48" s="14"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
     </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="40" x14ac:dyDescent="0.2">
       <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
+      <c r="B49" s="14" t="s">
+        <v>88</v>
+      </c>
       <c r="C49" s="14"/>
     </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="20" x14ac:dyDescent="0.2">
       <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
+      <c r="B50" s="14" t="s">
+        <v>89</v>
+      </c>
       <c r="C50" s="14"/>
     </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="40" x14ac:dyDescent="0.2">
       <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A52" s="14"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
     </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
     </row>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A54" s="14"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
     </row>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A55" s="14"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
     </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A56" s="14"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
     </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A57" s="14"/>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
     </row>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A58" s="14"/>
       <c r="B58" s="14"/>
       <c r="C58" s="14"/>
     </row>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A59" s="14"/>
       <c r="B59" s="14"/>
       <c r="C59" s="14"/>
     </row>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A60" s="14"/>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
     </row>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A61" s="14"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
     </row>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A62" s="14"/>
       <c r="B62" s="14"/>
       <c r="C62" s="14"/>
     </row>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A63" s="14"/>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
     </row>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A64" s="14"/>
       <c r="B64" s="14"/>
       <c r="C64" s="14"/>
     </row>
-    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A65" s="14"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
     </row>
-    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A66" s="14"/>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
     </row>
-    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A67" s="14"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
     </row>
-    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A68" s="14"/>
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
     </row>
-    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A69" s="14"/>
       <c r="B69" s="14"/>
       <c r="C69" s="14"/>
     </row>
-    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A70" s="14"/>
       <c r="B70" s="14"/>
       <c r="C70" s="14"/>
     </row>
-    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A71" s="14"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
     </row>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A72" s="14"/>
       <c r="B72" s="14"/>
       <c r="C72" s="14"/>
     </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
     </row>
-    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="5"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
     </row>
-    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="5"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
     </row>
-    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="5"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
     </row>
-    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="5"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
     </row>
-    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="5"/>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
     </row>
-    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="5"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
     </row>
-    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="5"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
     </row>
-    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="5"/>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
     </row>
-    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="5"/>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
     </row>
-    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="5"/>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
     </row>
-    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="5"/>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
     </row>
-    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="5"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
     </row>
-    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="5"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
     </row>
-    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="5"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
     </row>
-    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="5"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
     </row>
-    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
     </row>
-    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="5"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
     </row>
-    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="5"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
     </row>
-    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="5"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
     </row>
-    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="5"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
     </row>
-    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="5"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
     </row>
-    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="5"/>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
     </row>
-    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="5"/>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
     </row>
-    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="5"/>
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
     </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="5"/>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
     </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="5"/>
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
     </row>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="5"/>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
     </row>
-    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="5"/>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
     </row>
-    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="5"/>
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
     </row>
-    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
     </row>
-    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="5"/>
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
     </row>
-    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
     </row>
-    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="5"/>
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
     </row>
-    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
     </row>
-    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="5"/>
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
     </row>
-    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
     </row>
-    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="5"/>
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
     </row>
-    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
     </row>
-    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="5"/>
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
     </row>
-    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
     </row>
-    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="5"/>
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
     </row>
-    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="5"/>
       <c r="B115" s="5"/>
       <c r="C115" s="5"/>
     </row>
-    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="5"/>
       <c r="B116" s="5"/>
       <c r="C116" s="5"/>
     </row>
-    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="5"/>
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
     </row>
-    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="5"/>
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
     </row>
-    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="5"/>
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
     </row>
-    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="5"/>
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
     </row>
-    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="5"/>
       <c r="B121" s="5"/>
       <c r="C121" s="5"/>
     </row>
-    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="5"/>
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
     </row>
-    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="5"/>
       <c r="B123" s="5"/>
       <c r="C123" s="5"/>
     </row>
-    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="5"/>
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
     </row>
-    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="5"/>
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
     </row>
-    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="5"/>
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
     </row>
-    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="5"/>
       <c r="B127" s="5"/>
       <c r="C127" s="5"/>
     </row>
-    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="5"/>
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
     </row>
-    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="5"/>
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
     </row>
-    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="5"/>
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
     </row>
-    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="5"/>
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
     </row>
-    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="5"/>
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
     </row>
-    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="5"/>
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
     </row>
-    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="5"/>
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
     </row>
-    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="5"/>
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
     </row>
-    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="5"/>
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
     </row>
-    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="5"/>
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
     </row>
-    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="5"/>
       <c r="B138" s="5"/>
       <c r="C138" s="5"/>
     </row>
-    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="5"/>
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
     </row>
-    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="5"/>
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
     </row>
-    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="5"/>
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
     </row>
-    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="5"/>
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
     </row>
-    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="5"/>
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
     </row>
-    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="5"/>
       <c r="B144" s="5"/>
       <c r="C144" s="5"/>
     </row>
-    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="5"/>
       <c r="B145" s="5"/>
       <c r="C145" s="5"/>
     </row>
-    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" s="5"/>
       <c r="B146" s="5"/>
       <c r="C146" s="5"/>
     </row>
-    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="5"/>
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
     </row>
-    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="5"/>
       <c r="B148" s="5"/>
       <c r="C148" s="5"/>
     </row>
-    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="5"/>
       <c r="B149" s="5"/>
       <c r="C149" s="5"/>
     </row>
-    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="5"/>
       <c r="B150" s="5"/>
       <c r="C150" s="5"/>
     </row>
-    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="5"/>
       <c r="B151" s="5"/>
       <c r="C151" s="5"/>
     </row>
-    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="5"/>
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
     </row>
-    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="5"/>
       <c r="B153" s="5"/>
       <c r="C153" s="5"/>
     </row>
-    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="5"/>
       <c r="B154" s="5"/>
       <c r="C154" s="5"/>
     </row>
-    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="5"/>
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
     </row>
-    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" s="5"/>
       <c r="B156" s="5"/>
       <c r="C156" s="5"/>
     </row>
-    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="5"/>
       <c r="B157" s="5"/>
       <c r="C157" s="5"/>
     </row>
-    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="5"/>
       <c r="B158" s="5"/>
       <c r="C158" s="5"/>
     </row>
-    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="5"/>
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
     </row>
-    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" s="5"/>
       <c r="B160" s="5"/>
       <c r="C160" s="5"/>
     </row>
-    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" s="5"/>
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
     </row>
-    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A162" s="5"/>
       <c r="B162" s="5"/>
       <c r="C162" s="5"/>
     </row>
-    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A163" s="5"/>
       <c r="B163" s="5"/>
       <c r="C163" s="5"/>
     </row>
-    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="5"/>
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
     </row>
-    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A165" s="5"/>
       <c r="B165" s="5"/>
       <c r="C165" s="5"/>
     </row>
-    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A166" s="5"/>
       <c r="B166" s="5"/>
       <c r="C166" s="5"/>
     </row>
-    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A167" s="5"/>
       <c r="B167" s="5"/>
       <c r="C167" s="5"/>
     </row>
-    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A168" s="5"/>
       <c r="B168" s="5"/>
       <c r="C168" s="5"/>
     </row>
-    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="5"/>
       <c r="B169" s="5"/>
       <c r="C169" s="5"/>
     </row>
-    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A170" s="5"/>
       <c r="B170" s="5"/>
       <c r="C170" s="5"/>
     </row>
-    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A171" s="5"/>
       <c r="B171" s="5"/>
       <c r="C171" s="5"/>
     </row>
-    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" s="5"/>
       <c r="B172" s="5"/>
       <c r="C172" s="5"/>
     </row>
-    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A173" s="5"/>
       <c r="B173" s="5"/>
       <c r="C173" s="5"/>
     </row>
-    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A174" s="5"/>
       <c r="B174" s="5"/>
       <c r="C174" s="5"/>
     </row>
-    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A175" s="5"/>
       <c r="B175" s="5"/>
       <c r="C175" s="5"/>
     </row>
-    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A176" s="5"/>
       <c r="B176" s="5"/>
       <c r="C176" s="5"/>
     </row>
-    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" s="4"/>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
     </row>
-    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A178" s="4"/>
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
     </row>
-    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A179" s="4"/>
       <c r="B179" s="4"/>
       <c r="C179" s="4"/>
     </row>
-    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A180" s="4"/>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
     </row>
-    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A181" s="4"/>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
     </row>
-    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A182" s="4"/>
       <c r="B182" s="4"/>
       <c r="C182" s="4"/>
     </row>
-    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A183" s="7"/>
       <c r="B183" s="7"/>
       <c r="C183" s="7"/>
     </row>
-    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A184" s="7"/>
       <c r="B184" s="7"/>
       <c r="C184" s="7"/>
     </row>
-    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A185" s="7"/>
       <c r="B185" s="7"/>
       <c r="C185" s="7"/>
     </row>
-    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A186" s="7"/>
       <c r="B186" s="7"/>
       <c r="C186" s="7"/>
     </row>
-    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A187" s="7"/>
       <c r="B187" s="7"/>
       <c r="C187" s="7"/>
     </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A188" s="7"/>
       <c r="B188" s="7"/>
       <c r="C188" s="7"/>
     </row>
-    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A189" s="7"/>
       <c r="B189" s="7"/>
       <c r="C189" s="7"/>
     </row>
-    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A190" s="7"/>
       <c r="B190" s="7"/>
       <c r="C190" s="7"/>
     </row>
-    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A191" s="7"/>
       <c r="B191" s="7"/>
       <c r="C191" s="7"/>
     </row>
-    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A192" s="7"/>
       <c r="B192" s="7"/>
       <c r="C192" s="7"/>
     </row>
-    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A193" s="7"/>
       <c r="B193" s="7"/>
       <c r="C193" s="7"/>
     </row>
-    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A194" s="7"/>
       <c r="B194" s="7"/>
       <c r="C194" s="7"/>
     </row>
-    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A195" s="7"/>
       <c r="B195" s="7"/>
       <c r="C195" s="7"/>
     </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A196" s="7"/>
       <c r="B196" s="7"/>
       <c r="C196" s="7"/>
     </row>
-    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A197" s="7"/>
       <c r="B197" s="7"/>
       <c r="C197" s="7"/>
     </row>
-    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A198" s="7"/>
       <c r="B198" s="7"/>
       <c r="C198" s="7"/>
     </row>
-    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A199" s="7"/>
       <c r="B199" s="7"/>
       <c r="C199" s="7"/>
     </row>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A200" s="7"/>
       <c r="B200" s="7"/>
       <c r="C200" s="7"/>
     </row>
-    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A201" s="7"/>
       <c r="B201" s="7"/>
       <c r="C201" s="7"/>
     </row>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A202" s="7"/>
       <c r="B202" s="7"/>
       <c r="C202" s="7"/>
     </row>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A203" s="7"/>
       <c r="B203" s="7"/>
       <c r="C203" s="7"/>
     </row>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>